<commit_message>
more gas exchange potentially for lom jap and bolpor
</commit_message>
<xml_diff>
--- a/extras/sela_all_data.xlsx
+++ b/extras/sela_all_data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7230" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7230" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'ALL raw'!$A$1:$N$101</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -402,7 +402,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -864,50 +864,50 @@
     </xf>
   </cellXfs>
   <cellStyles count="44">
-    <cellStyle name="20% - Accent1 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="20% - Accent2 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="20% - Accent3 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="20% - Accent4 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="20% - Accent5 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="20% - Accent6 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="40% - Accent1 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="40% - Accent2 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="40% - Accent3 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="40% - Accent4 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="40% - Accent5 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="40% - Accent6 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="60% - Accent1 2" xfId="13" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="60% - Accent2 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="60% - Accent3 2" xfId="15" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="60% - Accent4 2" xfId="16" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="60% - Accent5 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="60% - Accent6 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="Accent1 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="Accent2 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
-    <cellStyle name="Accent3 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
-    <cellStyle name="Accent4 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="Accent5 2" xfId="23" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="Accent6 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="Bad 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="Calculation 2" xfId="26" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="Check Cell 2" xfId="27" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="Explanatory Text 2" xfId="28" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="Good 2" xfId="29" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="Heading 1 2" xfId="30" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="Heading 2 2" xfId="31" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="Heading 3 2" xfId="32" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="Heading 4 2" xfId="33" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="Input 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="Linked Cell 2" xfId="35" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="Neutral 2" xfId="36" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="20% - Accent1 2" xfId="1"/>
+    <cellStyle name="20% - Accent2 2" xfId="2"/>
+    <cellStyle name="20% - Accent3 2" xfId="3"/>
+    <cellStyle name="20% - Accent4 2" xfId="4"/>
+    <cellStyle name="20% - Accent5 2" xfId="5"/>
+    <cellStyle name="20% - Accent6 2" xfId="6"/>
+    <cellStyle name="40% - Accent1 2" xfId="7"/>
+    <cellStyle name="40% - Accent2 2" xfId="8"/>
+    <cellStyle name="40% - Accent3 2" xfId="9"/>
+    <cellStyle name="40% - Accent4 2" xfId="10"/>
+    <cellStyle name="40% - Accent5 2" xfId="11"/>
+    <cellStyle name="40% - Accent6 2" xfId="12"/>
+    <cellStyle name="60% - Accent1 2" xfId="13"/>
+    <cellStyle name="60% - Accent2 2" xfId="14"/>
+    <cellStyle name="60% - Accent3 2" xfId="15"/>
+    <cellStyle name="60% - Accent4 2" xfId="16"/>
+    <cellStyle name="60% - Accent5 2" xfId="17"/>
+    <cellStyle name="60% - Accent6 2" xfId="18"/>
+    <cellStyle name="Accent1 2" xfId="19"/>
+    <cellStyle name="Accent2 2" xfId="20"/>
+    <cellStyle name="Accent3 2" xfId="21"/>
+    <cellStyle name="Accent4 2" xfId="22"/>
+    <cellStyle name="Accent5 2" xfId="23"/>
+    <cellStyle name="Accent6 2" xfId="24"/>
+    <cellStyle name="Bad 2" xfId="25"/>
+    <cellStyle name="Calculation 2" xfId="26"/>
+    <cellStyle name="Check Cell 2" xfId="27"/>
+    <cellStyle name="Explanatory Text 2" xfId="28"/>
+    <cellStyle name="Good 2" xfId="29"/>
+    <cellStyle name="Heading 1 2" xfId="30"/>
+    <cellStyle name="Heading 2 2" xfId="31"/>
+    <cellStyle name="Heading 3 2" xfId="32"/>
+    <cellStyle name="Heading 4 2" xfId="33"/>
+    <cellStyle name="Input 2" xfId="34"/>
+    <cellStyle name="Linked Cell 2" xfId="35"/>
+    <cellStyle name="Neutral 2" xfId="36"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="Normal_Sheet1" xfId="38" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="Note 2" xfId="39" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="Output 2" xfId="40" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="Title 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
-    <cellStyle name="Total 2" xfId="42" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="Warning Text 2" xfId="43" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Normal 2" xfId="37"/>
+    <cellStyle name="Normal_Sheet1" xfId="38"/>
+    <cellStyle name="Note 2" xfId="39"/>
+    <cellStyle name="Output 2" xfId="40"/>
+    <cellStyle name="Title 2" xfId="41"/>
+    <cellStyle name="Total 2" xfId="42"/>
+    <cellStyle name="Warning Text 2" xfId="43"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
@@ -5104,23 +5104,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -5156,23 +5139,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5348,7 +5314,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5372,11 +5338,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P101"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" zoomScale="75" workbookViewId="0">
-      <selection activeCell="P47" sqref="P47"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="75" workbookViewId="0">
+      <selection activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8971,7 +8937,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N101" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:N101"/>
   <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8979,7 +8945,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
@@ -9850,7 +9816,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10046,7 +10012,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
@@ -10304,10 +10270,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
@@ -10720,7 +10686,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>